<commit_message>
small changes to graph
</commit_message>
<xml_diff>
--- a/models/data_set1/set1_models_comparison.xlsx
+++ b/models/data_set1/set1_models_comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christer\Python_projects\B.S.-Thesis\models\data_set6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christer\Python_projects\B.S.-Thesis\models\data_set1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CB2A7F-8E03-4495-9BC2-912230CE455A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277D98A6-3E2C-4DB1-A02D-F5B5D17F5AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31590" yWindow="525" windowWidth="20445" windowHeight="14115" xr2:uid="{ABE95A68-2D0F-42A7-8ED6-86D788EDBEAB}"/>
+    <workbookView xWindow="5715" yWindow="1755" windowWidth="20430" windowHeight="14115" xr2:uid="{ABE95A68-2D0F-42A7-8ED6-86D788EDBEAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,12 +58,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>MAE</t>
   </si>
   <si>
     <t>diff</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>line</t>
   </si>
 </sst>
 </file>
@@ -151,7 +157,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -170,6 +176,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$I$2:$M$2</c:f>
@@ -209,32 +236,329 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="1057531184"/>
         <c:axId val="1057533680"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>line</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.15407425357429821"/>
+                  <c:y val="-3.009241032370958E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Average = 16.05</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-SE"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.50536304156516632"/>
+                      <c:h val="9.7152960046660811E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-61A1-4E2C-B49C-6AE531CEDE5D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16.047510149071226</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.047510149071226</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.047510149071226</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.047510149071226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.047510149071226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-61A1-4E2C-B49C-6AE531CEDE5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1057531184"/>
+        <c:axId val="1057533680"/>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="1057531184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fi-FI"/>
+                  <a:t>Model</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-SE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-SE"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1057533680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1057533680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="10"/>
+          <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1270,15 +1594,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEAF74F-599C-45DC-A89F-88105B6B675F}">
-  <dimension ref="A1:M194"/>
+  <dimension ref="A1:R194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1297,7 +1621,7 @@
       <c r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
       <c r="I1">
@@ -1315,8 +1639,14 @@
       <c r="M1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>112.396484375</v>
       </c>
@@ -1352,8 +1682,18 @@
         <f t="array" ref="M2">SUMPRODUCT(ABS(B2:B194))/COUNT(B2:B194)</f>
         <v>17.497210547096348</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>AVERAGE(I2:M2)</f>
+        <v>16.047510149071226</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>9.7575607299804119</v>
       </c>
@@ -1369,8 +1709,14 @@
       <c r="F3">
         <v>25.109992980957003</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="R3">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>-6.4032897949218039</v>
       </c>
@@ -1386,8 +1732,11 @@
       <c r="F4">
         <v>4.6604385375976989</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>-20.892845153809006</v>
       </c>
@@ -1403,8 +1752,11 @@
       <c r="F5">
         <v>-5.0528182983400001</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>9.8274230956995723E-2</v>
       </c>
@@ -1420,8 +1772,11 @@
       <c r="F6">
         <v>1.9209861755371023</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>-11.860763549805</v>
       </c>
@@ -1437,8 +1792,11 @@
       <c r="F7">
         <v>-14.762329101562983</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>13.893417358397997</v>
       </c>
@@ -1454,8 +1812,11 @@
       <c r="F8">
         <v>25.5498046875</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>16.047510149071226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.361343383789062</v>
       </c>
@@ -1472,7 +1833,7 @@
         <v>-0.78188323974609297</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>-6.2834625244140057</v>
       </c>
@@ -1489,7 +1850,7 @@
         <v>-5.7551498413090059</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>346.84626770019469</v>
       </c>
@@ -1506,7 +1867,7 @@
         <v>163.88380432128901</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>-118.78606414794891</v>
       </c>
@@ -1523,7 +1884,7 @@
         <v>-111.33699798583891</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>-57.406311035156989</v>
       </c>
@@ -1540,7 +1901,7 @@
         <v>-38.337112426758011</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>12.485847473143991</v>
       </c>
@@ -1557,7 +1918,7 @@
         <v>12.543052673338991</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>19.186157226561988</v>
       </c>
@@ -1574,7 +1935,7 @@
         <v>15.280120849609006</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>-0.56013488769529829</v>
       </c>

</xml_diff>